<commit_message>
updated teaching and grades
</commit_message>
<xml_diff>
--- a/Advanced Reactor Materials/grading.xlsx
+++ b/Advanced Reactor Materials/grading.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beelbw/projects/TEACHING/Advanced Reactor Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBAB041-7A91-254D-8321-C4A3F9030AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E67733-B3C8-4C4D-98E1-A445866490BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="3820" windowWidth="28040" windowHeight="17440" xr2:uid="{142DFFB4-4F83-5448-8A86-CBCBD31FE822}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Grading for NE-795-010</t>
   </si>
@@ -94,19 +94,41 @@
   </si>
   <si>
     <t>Bonus</t>
+  </si>
+  <si>
+    <t>Penalty</t>
+  </si>
+  <si>
+    <t>A+ 98-100; A 93-97; A- 90-92</t>
+  </si>
+  <si>
+    <t>B+ 87-89; B 83-87; B- 80-82</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +151,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,25 +470,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97299AD9-D8EA-E746-928C-2071F09E3E0E}">
-  <dimension ref="B2:P19"/>
+  <dimension ref="B2:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -499,10 +523,13 @@
         <v>11</v>
       </c>
       <c r="O7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -526,14 +553,27 @@
       <c r="I8">
         <v>100</v>
       </c>
+      <c r="J8">
+        <v>93</v>
+      </c>
+      <c r="K8">
+        <f>J8+5</f>
+        <v>98</v>
+      </c>
       <c r="L8">
         <v>96</v>
       </c>
       <c r="M8">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N8" s="2">
+        <v>95</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>3</v>
       </c>
@@ -557,14 +597,30 @@
       <c r="I9">
         <v>91</v>
       </c>
+      <c r="J9">
+        <v>90</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K10" si="2">J9+5</f>
+        <v>95</v>
+      </c>
       <c r="L9">
         <v>96</v>
       </c>
       <c r="M9">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N9" s="2">
+        <v>95</v>
+      </c>
+      <c r="O9">
+        <v>10</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>2</v>
       </c>
@@ -588,63 +644,79 @@
       <c r="I10">
         <v>100</v>
       </c>
+      <c r="J10">
+        <v>96</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>101</v>
+      </c>
       <c r="L10">
         <v>97</v>
       </c>
       <c r="M10">
         <v>98</v>
       </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N10" s="2">
+        <v>95</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>15</v>
       </c>
       <c r="D12">
-        <f>AVERAGE(D8:D10)</f>
+        <f t="shared" ref="D12:I12" si="3">AVERAGE(D8:D10)</f>
         <v>90.333333333333329</v>
       </c>
       <c r="E12">
-        <f>AVERAGE(E8:E10)</f>
+        <f t="shared" si="3"/>
         <v>95.333333333333329</v>
       </c>
       <c r="F12">
-        <f>AVERAGE(F8:F10)</f>
+        <f t="shared" si="3"/>
         <v>90.333333333333329</v>
       </c>
       <c r="G12">
-        <f>AVERAGE(G8:G10)</f>
+        <f t="shared" si="3"/>
         <v>93.333333333333329</v>
       </c>
       <c r="H12">
-        <f>AVERAGE(H8:H10)</f>
+        <f t="shared" si="3"/>
         <v>92</v>
       </c>
       <c r="I12">
-        <f>AVERAGE(I8:I10)</f>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="J12" t="e">
-        <f t="shared" ref="J12:N12" si="2">AVERAGE(J8:J10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K12" t="e">
-        <f t="shared" ref="K12" si="3">AVERAGE(K8:K10)</f>
-        <v>#DIV/0!</v>
+      <c r="J12">
+        <f t="shared" ref="J12:N12" si="4">AVERAGE(J8:J10)</f>
+        <v>93</v>
+      </c>
+      <c r="K12">
+        <f>AVERAGE(K8:K10)</f>
+        <v>98</v>
       </c>
       <c r="L12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>96.333333333333329</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>98</v>
       </c>
-      <c r="N12" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="N12">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>12</v>
       </c>
@@ -681,17 +753,16 @@
       <c r="N13">
         <v>20</v>
       </c>
-      <c r="P13">
-        <f>SUM(E13,G13:N13)</f>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P15" t="s">
+      <c r="O13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>12.5</v>
       </c>
@@ -699,6 +770,9 @@
         <v>12.5</v>
       </c>
       <c r="I16">
+        <v>12.5</v>
+      </c>
+      <c r="K16">
         <v>12.5</v>
       </c>
       <c r="L16">
@@ -707,12 +781,15 @@
       <c r="M16">
         <v>15</v>
       </c>
-      <c r="P16">
-        <f>SUM(D16:N16)</f>
-        <v>67.5</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <v>20</v>
+      </c>
+      <c r="Q16">
+        <f>SUM(D16:O16)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>4</v>
       </c>
@@ -730,7 +807,7 @@
       </c>
       <c r="K17">
         <f>K8*K$13/100</f>
-        <v>0</v>
+        <v>12.25</v>
       </c>
       <c r="L17">
         <f>L8*L$13/100</f>
@@ -740,12 +817,16 @@
         <f>M8*M$13/100</f>
         <v>14.7</v>
       </c>
-      <c r="P17" s="1">
-        <f>SUM(D17:N17)/$P$16</f>
-        <v>0.96444444444444433</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <f>(N8-O8)*O$13/100</f>
+        <v>18</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>SUM(D17:O17)/$Q$16</f>
+        <v>0.9534999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -763,22 +844,26 @@
       </c>
       <c r="K18">
         <f>K9*K$13/100</f>
-        <v>0</v>
+        <v>11.875</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:M19" si="4">L9*L$13/100</f>
+        <f t="shared" ref="L18:M19" si="5">L9*L$13/100</f>
         <v>14.4</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.7</v>
       </c>
-      <c r="P18" s="1">
-        <f>SUM(D18:N18)/$P$16</f>
-        <v>0.931111111111111</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <f t="shared" ref="O18:O19" si="6">(N9-O9)*O$13/100</f>
+        <v>17</v>
+      </c>
+      <c r="Q18" s="1">
+        <f t="shared" ref="Q18:Q19" si="7">SUM(D18:O18)/$Q$16</f>
+        <v>0.9172499999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>2</v>
       </c>
@@ -796,19 +881,23 @@
       </c>
       <c r="K19">
         <f>K10*K$13/100</f>
-        <v>0</v>
+        <v>12.625</v>
       </c>
       <c r="L19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.55</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.7</v>
       </c>
-      <c r="P19" s="1">
-        <f t="shared" ref="P19" si="5">SUM(D19:N19)/$P$16</f>
-        <v>0.98703703703703705</v>
+      <c r="O19">
+        <f t="shared" si="6"/>
+        <v>18</v>
+      </c>
+      <c r="Q19" s="1">
+        <f t="shared" si="7"/>
+        <v>0.97250000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
end of fall 2021
</commit_message>
<xml_diff>
--- a/Advanced Reactor Materials/grading.xlsx
+++ b/Advanced Reactor Materials/grading.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beelbw/projects/TEACHING/Advanced Reactor Materials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminbeeler/projects/TEACHING/Advanced Reactor Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E67733-B3C8-4C4D-98E1-A445866490BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F837046-1BB8-2E4C-9F68-69D0B9C227B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3340" yWindow="3820" windowWidth="28040" windowHeight="17440" xr2:uid="{142DFFB4-4F83-5448-8A86-CBCBD31FE822}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>Quiz #4 *</t>
   </si>
   <si>
-    <t>Bonus</t>
-  </si>
-  <si>
     <t>Penalty</t>
   </si>
   <si>
@@ -103,23 +100,19 @@
   </si>
   <si>
     <t>B+ 87-89; B 83-87; B- 80-82</t>
+  </si>
+  <si>
+    <t>Curve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,7 +148,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,7 +466,7 @@
   <dimension ref="B2:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -523,10 +516,10 @@
         <v>11</v>
       </c>
       <c r="O7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.2">
@@ -566,11 +559,14 @@
       <c r="M8">
         <v>98</v>
       </c>
-      <c r="N8" s="2">
-        <v>95</v>
+      <c r="N8" s="3">
+        <v>85</v>
       </c>
       <c r="O8">
         <v>5</v>
+      </c>
+      <c r="P8">
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.2">
@@ -610,14 +606,17 @@
       <c r="M9">
         <v>98</v>
       </c>
-      <c r="N9" s="2">
-        <v>95</v>
+      <c r="N9" s="3">
+        <v>75</v>
       </c>
       <c r="O9">
+        <v>15</v>
+      </c>
+      <c r="P9">
         <v>10</v>
       </c>
-      <c r="Q9" s="3" t="s">
-        <v>21</v>
+      <c r="Q9" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.2">
@@ -657,14 +656,17 @@
       <c r="M10">
         <v>98</v>
       </c>
-      <c r="N10" s="2">
-        <v>95</v>
+      <c r="N10" s="3">
+        <v>85</v>
       </c>
       <c r="O10">
         <v>5</v>
       </c>
-      <c r="Q10" s="3" t="s">
-        <v>22</v>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:17" x14ac:dyDescent="0.2">
@@ -713,7 +715,15 @@
       </c>
       <c r="N12">
         <f t="shared" si="4"/>
-        <v>95</v>
+        <v>81.666666666666671</v>
+      </c>
+      <c r="O12">
+        <f>N12-AVERAGE(O8:O10)</f>
+        <v>73.333333333333343</v>
+      </c>
+      <c r="P12">
+        <f>O12+AVERAGE(P8:P10)</f>
+        <v>83.333333333333343</v>
       </c>
     </row>
     <row r="13" spans="2:17" x14ac:dyDescent="0.2">
@@ -756,6 +766,9 @@
       <c r="O13">
         <v>20</v>
       </c>
+      <c r="P13">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.2">
       <c r="Q15" t="s">
@@ -781,11 +794,11 @@
       <c r="M16">
         <v>15</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>20</v>
       </c>
       <c r="Q16">
-        <f>SUM(D16:O16)</f>
+        <f>SUM(D16:P16)</f>
         <v>100</v>
       </c>
     </row>
@@ -817,12 +830,12 @@
         <f>M8*M$13/100</f>
         <v>14.7</v>
       </c>
-      <c r="O17">
-        <f>(N8-O8)*O$13/100</f>
+      <c r="P17">
+        <f>(N8-O8+P8)*P$13/100</f>
         <v>18</v>
       </c>
       <c r="Q17" s="1">
-        <f>SUM(D17:O17)/$Q$16</f>
+        <f>SUM(D17:P17)/$Q$16</f>
         <v>0.9534999999999999</v>
       </c>
     </row>
@@ -854,13 +867,13 @@
         <f t="shared" si="5"/>
         <v>14.7</v>
       </c>
-      <c r="O18">
-        <f t="shared" ref="O18:O19" si="6">(N9-O9)*O$13/100</f>
-        <v>17</v>
+      <c r="P18">
+        <f t="shared" ref="P18:P19" si="6">(N9-O9+P9)*P$13/100</f>
+        <v>14</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" ref="Q18:Q19" si="7">SUM(D18:O18)/$Q$16</f>
-        <v>0.9172499999999999</v>
+        <f t="shared" ref="Q18:Q19" si="7">SUM(D18:P18)/$Q$16</f>
+        <v>0.88724999999999998</v>
       </c>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.2">
@@ -891,7 +904,7 @@
         <f t="shared" si="5"/>
         <v>14.7</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f t="shared" si="6"/>
         <v>18</v>
       </c>

</xml_diff>